<commit_message>
Working on csv files creation from dataUploadApp. Modified ClinicalData_template and included CKG identifiers as new columns after upload of clinical data file.
</commit_message>
<xml_diff>
--- a/report_manager/apps/templates/ClinicalData_template.xlsx
+++ b/report_manager/apps/templates/ClinicalData_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plh450/Clinical_Proteomics/CKG/clinicalknowledgegraph/report_manager/apps/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5518FD5-FC72-3449-B7A0-1257EE5F11B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25278A-3D60-2A43-B0C1-8AF73EE51018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80240" yWindow="140" windowWidth="31140" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,6 @@
     <t>subject external_id</t>
   </si>
   <si>
-    <t>tissue id</t>
-  </si>
-  <si>
-    <t>intervention id</t>
-  </si>
-  <si>
-    <t>disease id</t>
-  </si>
-  <si>
     <t>biological_sample external_id</t>
   </si>
   <si>
@@ -143,6 +134,15 @@
   </si>
   <si>
     <t>procentfat</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>intervention</t>
+  </si>
+  <si>
+    <t>disease</t>
   </si>
 </sst>
 </file>
@@ -546,13 +546,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="44" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
@@ -560,124 +599,124 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified data upload to be more readable. Correcting Clinical data template fields
</commit_message>
<xml_diff>
--- a/report_manager/apps/templates/ClinicalData_template.xlsx
+++ b/report_manager/apps/templates/ClinicalData_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plh450/Clinical_Proteomics/CKG/clinicalknowledgegraph/report_manager/apps/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25278A-3D60-2A43-B0C1-8AF73EE51018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C89E56B-D3AB-054C-989D-4A0C2E670B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80240" yWindow="140" windowWidth="31140" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>subject external_id</t>
   </si>
@@ -85,57 +85,6 @@
     <t>grouping2</t>
   </si>
   <si>
-    <t>Body weight</t>
-  </si>
-  <si>
-    <t>Body mass index</t>
-  </si>
-  <si>
-    <t>Waist circumference</t>
-  </si>
-  <si>
-    <t>Cholesterol level</t>
-  </si>
-  <si>
-    <t>Waist/hip ratio</t>
-  </si>
-  <si>
-    <t>Tobacco smoking behavior - finding</t>
-  </si>
-  <si>
-    <t>Plasma LDL cholesterol leve</t>
-  </si>
-  <si>
-    <t>Plasma HDL cholesterol measurement</t>
-  </si>
-  <si>
-    <t>Hyperpiesis</t>
-  </si>
-  <si>
-    <t>Diastolic blood pressure</t>
-  </si>
-  <si>
-    <t>Gluten specific IgE antibody measurement (procedure)</t>
-  </si>
-  <si>
-    <t>Ordinal level of hemoglobin A1c (observable entity)</t>
-  </si>
-  <si>
-    <t>h.dexa</t>
-  </si>
-  <si>
-    <t>w.dexa</t>
-  </si>
-  <si>
-    <t>Body fat</t>
-  </si>
-  <si>
-    <t>totalmass</t>
-  </si>
-  <si>
-    <t>procentfat</t>
-  </si>
-  <si>
     <t>tissue</t>
   </si>
   <si>
@@ -143,6 +92,84 @@
   </si>
   <si>
     <t>disease</t>
+  </si>
+  <si>
+    <t>date of T2D diagnosis</t>
+  </si>
+  <si>
+    <t>Biological sex (property) (qualifier value) (734000001)</t>
+  </si>
+  <si>
+    <t>Age (102518004)</t>
+  </si>
+  <si>
+    <t>Body height (50373000)</t>
+  </si>
+  <si>
+    <t>Weight (property) (qualifier value) (726527001)</t>
+  </si>
+  <si>
+    <t>Body mass index (60621009)</t>
+  </si>
+  <si>
+    <t>Systole (111973004)</t>
+  </si>
+  <si>
+    <t>Diastole (90892000)</t>
+  </si>
+  <si>
+    <t>Waist circumference (276361009)</t>
+  </si>
+  <si>
+    <t>Drug therapy (procedure) (416608005)</t>
+  </si>
+  <si>
+    <t>Lipid-lowering therapy (134350008)</t>
+  </si>
+  <si>
+    <t>NAFLD score</t>
+  </si>
+  <si>
+    <t>Fasting blood glucose level (271062006)</t>
+  </si>
+  <si>
+    <t>platelets/liter (277200003)</t>
+  </si>
+  <si>
+    <t>Bilirubin level (302787001)</t>
+  </si>
+  <si>
+    <t>Albumin measurement (26758005)</t>
+  </si>
+  <si>
+    <t>Alanine aminotransferase measurement (34608000)</t>
+  </si>
+  <si>
+    <t>Aspartate aminotransferase measurement (45896001)</t>
+  </si>
+  <si>
+    <t>Alkaline phosphatase measurement (88810008)</t>
+  </si>
+  <si>
+    <t>Gamma glutamyl transferase measurement (69480007)</t>
+  </si>
+  <si>
+    <t>Hemoglobin A1c measurement (43396009)</t>
+  </si>
+  <si>
+    <t>Total cholesterol:HDL ratio measurement (166842003)</t>
+  </si>
+  <si>
+    <t>High density lipoprotein measurement (17888004)</t>
+  </si>
+  <si>
+    <t>Low density lipoprotein cholesterol measurement (113079009)</t>
+  </si>
+  <si>
+    <t>VLDL cholesterol measurement (104585005)</t>
+  </si>
+  <si>
+    <t>Triglycerides measurement (14740000)</t>
   </si>
 </sst>
 </file>
@@ -158,9 +185,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,27 +200,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -203,9 +214,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,68 +553,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="44" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="44" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="44" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="44" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -668,56 +687,104 @@
         <v>20</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="10" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>